<commit_message>
added website link icon
if website is present in associated data table
</commit_message>
<xml_diff>
--- a/Quasar Members.xlsx
+++ b/Quasar Members.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmhooym\GitHub\quasarcollaboration.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F286CC66-A841-44EB-9A05-C999ABE28F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F6F851-4728-4075-83A4-5FC04E36284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current members" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="133">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -417,13 +417,28 @@
   </si>
   <si>
     <t>c.martinezharris@qut.edu.au</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>https://hughmcdougall.github.io/</t>
+  </si>
+  <si>
+    <t>https://mitchellhooymans.com</t>
+  </si>
+  <si>
+    <t>https://rebeccamcelroy.github.io</t>
+  </si>
+  <si>
+    <t>https://mjcowley.github.io</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -452,6 +467,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -470,10 +492,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -486,8 +509,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -752,11 +777,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I2"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -769,10 +794,10 @@
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,11 +825,14 @@
       <c r="I1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -832,8 +860,9 @@
       <c r="I2" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -861,8 +890,9 @@
       <c r="I3" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -890,8 +920,9 @@
       <c r="I4" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -919,8 +950,9 @@
       <c r="I5" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -948,8 +980,9 @@
       <c r="I6" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -977,8 +1010,9 @@
       <c r="I7" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1006,8 +1040,9 @@
       <c r="I8" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1035,8 +1070,9 @@
       <c r="I9" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1064,8 +1100,11 @@
       <c r="I10" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1093,8 +1132,9 @@
       <c r="I11" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -1122,8 +1162,9 @@
       <c r="I12" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -1151,8 +1192,9 @@
       <c r="I13" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1180,8 +1222,9 @@
       <c r="I14" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1209,8 +1252,9 @@
       <c r="I15" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1238,8 +1282,11 @@
       <c r="I16" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1267,8 +1314,9 @@
       <c r="I17" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1296,8 +1344,9 @@
       <c r="I18" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -1325,8 +1374,9 @@
       <c r="I19" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -1354,8 +1404,9 @@
       <c r="I20" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1383,8 +1434,9 @@
       <c r="I21" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>71</v>
       </c>
@@ -1412,8 +1464,9 @@
       <c r="I22" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
@@ -1441,8 +1494,9 @@
       <c r="I23" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -1470,8 +1524,9 @@
       <c r="I24" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -1497,8 +1552,9 @@
         <v>13</v>
       </c>
       <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -1524,8 +1580,9 @@
         <v>13</v>
       </c>
       <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -1551,8 +1608,9 @@
         <v>13</v>
       </c>
       <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -1578,8 +1636,9 @@
         <v>13</v>
       </c>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -1605,8 +1664,9 @@
         <v>16</v>
       </c>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -1632,8 +1692,9 @@
         <v>13</v>
       </c>
       <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
@@ -1659,8 +1720,9 @@
         <v>16</v>
       </c>
       <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
@@ -1688,8 +1750,11 @@
       <c r="I32" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -1717,8 +1782,9 @@
       <c r="I33" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>58</v>
       </c>
@@ -1746,8 +1812,9 @@
       <c r="I34" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>59</v>
       </c>
@@ -1775,8 +1842,9 @@
       <c r="I35" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>60</v>
       </c>
@@ -1804,8 +1872,9 @@
       <c r="I36" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -1833,8 +1902,9 @@
       <c r="I37" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1862,8 +1932,9 @@
       <c r="I38" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
@@ -1891,8 +1962,9 @@
       <c r="I39" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>64</v>
       </c>
@@ -1920,8 +1992,9 @@
       <c r="I40" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>65</v>
       </c>
@@ -1949,8 +2022,9 @@
       <c r="I41" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>66</v>
       </c>
@@ -1978,8 +2052,11 @@
       <c r="I42" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>67</v>
       </c>
@@ -2007,8 +2084,9 @@
       <c r="I43" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>68</v>
       </c>
@@ -2036,8 +2114,9 @@
       <c r="I44" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>69</v>
       </c>
@@ -2065,8 +2144,9 @@
       <c r="I45" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>70</v>
       </c>
@@ -2094,8 +2174,9 @@
       <c r="I46" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>73</v>
       </c>
@@ -2123,8 +2204,9 @@
       <c r="I47" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>126</v>
       </c>
@@ -2152,6 +2234,7 @@
       <c r="I48" s="4" t="s">
         <v>127</v>
       </c>
+      <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
@@ -3028,25 +3111,31 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" sqref="F2 F3:F145" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F145" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"&lt;5 yr post PhD,5-10 yr post PhD,in PhD,&gt;10 yr post PhD,Honours student,Undergraduate,in MPhil"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2 C3:C145" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C145" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Brisbane,Toowoomba,Springfield,Remote"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2 E3:E145" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E145" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Exoplanets,Stars,Galaxies,Cosmology,Solar system,Astroparticle"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2 G3:G145" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G145" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Female,Male,Gender diverse"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2 D3:D145" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D145" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Staff,Student"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2 B3:B145" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B145" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"UQ,UniSQ,QUT"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J42" r:id="rId1" xr:uid="{3AB21A4F-2DF7-4799-9C59-2797C0F792D7}"/>
+    <hyperlink ref="J32" r:id="rId2" xr:uid="{571EDA3A-934B-46E6-8877-7B008EE00B1D}"/>
+    <hyperlink ref="J16" r:id="rId3" xr:uid="{27294F6D-2BDE-4E4E-8D62-68D959B8FC3E}"/>
+    <hyperlink ref="J10" r:id="rId4" xr:uid="{EB055170-13BD-40E3-A039-4A26E68960C4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>